<commit_message>
Fixed 2016 powerplant generation data
</commit_message>
<xml_diff>
--- a/src/tasks/task-01-satellite-data-extraction/Tamil_Nadu_PowerPlants_2013-2018.xlsx
+++ b/src/tasks/task-01-satellite-data-extraction/Tamil_Nadu_PowerPlants_2013-2018.xlsx
@@ -1,21 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Saurabh Shetty\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\GIT\Omdena\chennai-india-power-outage\src\tasks\task-01-satellite-data-extraction\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F6260282-9BA2-4658-BE02-4668E0A7A029}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{923B6B7D-C78C-4055-B7EC-3C251D99C8E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tamil_Nadu_PowerPlants" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -1204,16 +1216,16 @@
     <t>{"type":"Point","coordinates":[78.13740730608698,8.915885794677102]}</t>
   </si>
   <si>
-    <t>generation_gwh_2017</t>
-  </si>
-  <si>
-    <t>generation_gwh_2018</t>
+    <t>gwh_2017</t>
+  </si>
+  <si>
+    <t>gwh_2018</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -2047,16 +2059,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="P2" sqref="P2"/>
+    <sheetView tabSelected="1" topLeftCell="H16" workbookViewId="0">
+      <selection activeCell="P5" sqref="P5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="15" max="15" width="14.88671875" customWidth="1"/>
+    <col min="15" max="15" width="23.77734375" customWidth="1"/>
     <col min="16" max="16" width="20" customWidth="1"/>
     <col min="17" max="17" width="21.33203125" customWidth="1"/>
   </cols>
@@ -3726,7 +3738,7 @@
         <v>152.25296599999999</v>
       </c>
       <c r="O24">
-        <v>0</v>
+        <v>195.88466099999999</v>
       </c>
       <c r="P24">
         <v>0</v>
@@ -3794,7 +3806,7 @@
         <v>518.84400000000005</v>
       </c>
       <c r="O25">
-        <v>0</v>
+        <v>335.92700000000002</v>
       </c>
       <c r="P25">
         <v>309.54899999999998</v>
@@ -3862,7 +3874,7 @@
         <v>620.20699999999999</v>
       </c>
       <c r="O26">
-        <v>0</v>
+        <v>480.96699999999998</v>
       </c>
       <c r="P26">
         <v>469.44</v>
@@ -3930,7 +3942,7 @@
         <v>363.39800000000002</v>
       </c>
       <c r="O27">
-        <v>0</v>
+        <v>308.96699999999998</v>
       </c>
       <c r="P27">
         <v>266.15800000000002</v>
@@ -3998,7 +4010,7 @@
         <v>680.47500000000002</v>
       </c>
       <c r="O28">
-        <v>0</v>
+        <v>906.99599999999998</v>
       </c>
       <c r="P28">
         <v>1198.136</v>
@@ -4066,7 +4078,7 @@
         <v>170.73400000000001</v>
       </c>
       <c r="O29">
-        <v>0</v>
+        <v>374.892</v>
       </c>
       <c r="P29">
         <v>370.625</v>
@@ -4133,8 +4145,8 @@
       <c r="N30">
         <v>0</v>
       </c>
-      <c r="O30">
-        <v>0</v>
+      <c r="O30" t="e">
+        <v>#N/A</v>
       </c>
       <c r="P30" t="e">
         <v>#N/A</v>
@@ -4205,7 +4217,7 @@
         <v>8.2959124729978395</v>
       </c>
       <c r="O31">
-        <v>0</v>
+        <v>10.46898</v>
       </c>
       <c r="P31">
         <v>5.85771</v>
@@ -4273,7 +4285,7 @@
         <v>39.954000000000001</v>
       </c>
       <c r="O32">
-        <v>0</v>
+        <v>11.308044000000001</v>
       </c>
       <c r="P32">
         <v>0</v>
@@ -4411,8 +4423,8 @@
       <c r="N34">
         <v>347.36</v>
       </c>
-      <c r="O34">
-        <v>0</v>
+      <c r="O34" t="e">
+        <v>#N/A</v>
       </c>
       <c r="P34" t="e">
         <v>#N/A</v>
@@ -4483,7 +4495,7 @@
         <v>7130.5069999999996</v>
       </c>
       <c r="O35">
-        <v>0</v>
+        <v>8564.3790000000008</v>
       </c>
       <c r="P35">
         <v>6605.259</v>
@@ -4554,7 +4566,7 @@
         <v>4046.3939999999998</v>
       </c>
       <c r="O36">
-        <v>0</v>
+        <v>3365.7460000000001</v>
       </c>
       <c r="P36">
         <v>3824.1390000000001</v>
@@ -4625,7 +4637,7 @@
         <v>3000.0610000000001</v>
       </c>
       <c r="O37">
-        <v>0</v>
+        <v>3055.3049999999998</v>
       </c>
       <c r="P37">
         <v>2972.8139999999999</v>
@@ -4696,7 +4708,7 @@
         <v>1383.037</v>
       </c>
       <c r="O38">
-        <v>0</v>
+        <v>1002.6660000000001</v>
       </c>
       <c r="P38">
         <v>920.12900000000002</v>
@@ -4767,7 +4779,7 @@
         <v>9546.6479999999992</v>
       </c>
       <c r="O39">
-        <v>0</v>
+        <v>9987.7520000000004</v>
       </c>
       <c r="P39">
         <v>9246.0619999999999</v>
@@ -4838,7 +4850,7 @@
         <v>660.78</v>
       </c>
       <c r="O40">
-        <v>0</v>
+        <v>1128.2940000000001</v>
       </c>
       <c r="P40">
         <v>1687.0440000000001</v>
@@ -4909,7 +4921,7 @@
         <v>6501.3729999999996</v>
       </c>
       <c r="O41">
-        <v>0</v>
+        <v>5089.6549999999997</v>
       </c>
       <c r="P41">
         <v>4812.82</v>
@@ -4980,7 +4992,7 @@
         <v>728.36399999999901</v>
       </c>
       <c r="O42">
-        <v>0</v>
+        <v>21.730399999999999</v>
       </c>
       <c r="P42">
         <v>0</v>
@@ -5051,7 +5063,7 @@
         <v>3502.11</v>
       </c>
       <c r="O43">
-        <v>0</v>
+        <v>5806.8509999999997</v>
       </c>
       <c r="P43">
         <v>5026.3620000000001</v>
@@ -5122,7 +5134,7 @@
         <v>5471.3280000000004</v>
       </c>
       <c r="O44">
-        <v>0</v>
+        <v>5239.7030000000004</v>
       </c>
       <c r="P44">
         <v>4666.6719999999996</v>
@@ -5190,7 +5202,7 @@
         <v>115.98715</v>
       </c>
       <c r="O45">
-        <v>0</v>
+        <v>66.207300000000004</v>
       </c>
       <c r="P45">
         <v>114.70359999999999</v>
@@ -5258,7 +5270,7 @@
         <v>502.25609999999898</v>
       </c>
       <c r="O46">
-        <v>0</v>
+        <v>93.440449999999998</v>
       </c>
       <c r="P46">
         <v>285.66449999999998</v>
@@ -5326,7 +5338,7 @@
         <v>92.037499999999994</v>
       </c>
       <c r="O47">
-        <v>0</v>
+        <v>42.496450000000003</v>
       </c>
       <c r="P47">
         <v>70.336550000000003</v>
@@ -5462,7 +5474,7 @@
         <v>262.47104999999999</v>
       </c>
       <c r="O49">
-        <v>0</v>
+        <v>226.96944999999999</v>
       </c>
       <c r="P49">
         <v>156.94134999999901</v>
@@ -5530,7 +5542,7 @@
         <v>152.1952</v>
       </c>
       <c r="O50">
-        <v>0</v>
+        <v>61.421349999999997</v>
       </c>
       <c r="P50">
         <v>89.629599999999996</v>
@@ -5598,7 +5610,7 @@
         <v>410.56684999999999</v>
       </c>
       <c r="O51">
-        <v>0</v>
+        <v>287.943049999999</v>
       </c>
       <c r="P51">
         <v>382.43819999999999</v>
@@ -5666,7 +5678,7 @@
         <v>1365.5778</v>
       </c>
       <c r="O52">
-        <v>0</v>
+        <v>811.53195000000005</v>
       </c>
       <c r="P52">
         <v>802.19884999999999</v>
@@ -5734,7 +5746,7 @@
         <v>56.605550000000001</v>
       </c>
       <c r="O53">
-        <v>0</v>
+        <v>12.676299999999999</v>
       </c>
       <c r="P53">
         <v>0.97509999999999997</v>
@@ -5802,7 +5814,7 @@
         <v>279.15719999999999</v>
       </c>
       <c r="O54">
-        <v>0</v>
+        <v>191.58725000000001</v>
       </c>
       <c r="P54">
         <v>272.73944999999998</v>
@@ -5870,7 +5882,7 @@
         <v>222.25315000000001</v>
       </c>
       <c r="O55">
-        <v>0</v>
+        <v>91.80865</v>
       </c>
       <c r="P55">
         <v>131.29024999999999</v>
@@ -5938,7 +5950,7 @@
         <v>339.72284999999999</v>
       </c>
       <c r="O56">
-        <v>0</v>
+        <v>124.8526</v>
       </c>
       <c r="P56">
         <v>214.48220000000001</v>
@@ -6006,7 +6018,7 @@
         <v>2927</v>
       </c>
       <c r="O57">
-        <v>0</v>
+        <v>2916.67</v>
       </c>
       <c r="P57">
         <v>2704.38</v>
@@ -6497,7 +6509,7 @@
         <v>78.883600000000001</v>
       </c>
       <c r="O64">
-        <v>0</v>
+        <v>62.973549999999904</v>
       </c>
       <c r="P64">
         <v>85.032699999999906</v>
@@ -6565,7 +6577,7 @@
         <v>25.501849999999902</v>
       </c>
       <c r="O65">
-        <v>0</v>
+        <v>23.830249999999999</v>
       </c>
       <c r="P65">
         <v>26.974450000000001</v>
@@ -6633,7 +6645,7 @@
         <v>6.9948499999999996</v>
       </c>
       <c r="O66">
-        <v>0</v>
+        <v>19.730849999999901</v>
       </c>
       <c r="P66">
         <v>37.431899999999999</v>
@@ -6701,7 +6713,7 @@
         <v>155.72744999999901</v>
       </c>
       <c r="O67">
-        <v>0</v>
+        <v>20.48705</v>
       </c>
       <c r="P67">
         <v>16.8752</v>
@@ -6769,7 +6781,7 @@
         <v>5.6515999999999904</v>
       </c>
       <c r="O68">
-        <v>0</v>
+        <v>17.382649999999899</v>
       </c>
       <c r="P68">
         <v>0</v>
@@ -6837,7 +6849,7 @@
         <v>277.18709999999999</v>
       </c>
       <c r="O69">
-        <v>0</v>
+        <v>168.58285000000001</v>
       </c>
       <c r="P69">
         <v>123.3601</v>
@@ -7186,7 +7198,7 @@
         <v>2776.9470000000001</v>
       </c>
       <c r="O74">
-        <v>0</v>
+        <v>3256.8510000000001</v>
       </c>
       <c r="P74">
         <v>2939.8879999999999</v>
@@ -7257,7 +7269,7 @@
         <v>1057.8403000000001</v>
       </c>
       <c r="O75">
-        <v>0</v>
+        <v>4652.2794999999996</v>
       </c>
       <c r="P75">
         <v>5288.2</v>
@@ -7328,7 +7340,7 @@
         <v>3674.16</v>
       </c>
       <c r="O76">
-        <v>0</v>
+        <v>3212.7</v>
       </c>
       <c r="P76">
         <v>2273.06</v>
@@ -7399,7 +7411,7 @@
         <v>6031.9565000000002</v>
       </c>
       <c r="O77">
-        <v>0</v>
+        <v>5912.3959999999997</v>
       </c>
       <c r="P77">
         <v>5447.4696999999996</v>
@@ -7470,7 +7482,7 @@
         <v>2504.5300000000002</v>
       </c>
       <c r="O78">
-        <v>0</v>
+        <v>3482.79</v>
       </c>
       <c r="P78">
         <v>3630</v>

</xml_diff>